<commit_message>
changes to dms workflows and testing
</commit_message>
<xml_diff>
--- a/EA Waste Tonnage Returns/Documents/Config/config.xlsx
+++ b/EA Waste Tonnage Returns/Documents/Config/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>timeoutS</t>
   </si>
@@ -170,42 +170,12 @@
     <t>Home url site for DMS</t>
   </si>
   <si>
-    <t>https://defradev.sharepoint.com/sites/EADMSRoboticsHomeSite</t>
-  </si>
-  <si>
-    <t>https://defradev.sharepoint.com/sites/EADMSRobotics1/</t>
-  </si>
-  <si>
     <t>DMSSiteUrl</t>
   </si>
   <si>
     <t>Url for DMS site</t>
   </si>
   <si>
-    <t>DMSDocumentUrl</t>
-  </si>
-  <si>
-    <t>Url for where the document will be uploaded to</t>
-  </si>
-  <si>
-    <t>DMSReturnFolderUrl</t>
-  </si>
-  <si>
-    <t>Url for return folder on DMS</t>
-  </si>
-  <si>
-    <t>https://defradev.sharepoint.com/sites/EADMSRobotics1/LIB1/{0}/Returns</t>
-  </si>
-  <si>
-    <t>Compliance Waste Returns {0} {1}</t>
-  </si>
-  <si>
-    <t>Compliance Waste Returns {0} {1} - Email and Submission</t>
-  </si>
-  <si>
-    <t>/sites/EADMSRobotics1/LIB1/{0}/Returns/{1}</t>
-  </si>
-  <si>
     <t>EmailAccount</t>
   </si>
   <si>
@@ -213,6 +183,18 @@
   </si>
   <si>
     <t>Email account used for the emails being processed by the robot</t>
+  </si>
+  <si>
+    <t>Waste Return {0} {1}</t>
+  </si>
+  <si>
+    <t>Waste Return Correspondence {0} {1} - Email and Submission</t>
+  </si>
+  <si>
+    <t>https://defra.sharepoint.com/sites/EADMSProdhomesite</t>
+  </si>
+  <si>
+    <t>https://defra.sharepoint.com/sites/EADMSProd</t>
   </si>
 </sst>
 </file>
@@ -266,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -291,9 +273,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -344,8 +323,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C29" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C27" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C27"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Name" dataDxfId="2"/>
     <tableColumn id="2" name="Value" dataDxfId="1"/>
@@ -652,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,21 +841,21 @@
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>48</v>
+      <c r="B20" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>47</v>
@@ -884,89 +863,67 @@
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="C22" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
+    <row r="27" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>